<commit_message>
Finito l'esercizio aggiungendo gli attributi
</commit_message>
<xml_diff>
--- a/Tabella Auto.xlsx
+++ b/Tabella Auto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Desktop\Desktop\Programming\NET Course\repos\db-first\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07468985-2E15-4FB0-BA5D-7FD182E503A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40001_{31D00E0B-196D-4799-A899-FC748D7C3ADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
   <si>
     <t>Titolo:</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>PRIMARY KEY, CREATE INDEX</t>
+  </si>
+  <si>
+    <t>NOT NULL</t>
+  </si>
+  <si>
+    <t>NOT NULL, UNIQUE</t>
   </si>
 </sst>
 </file>
@@ -490,14 +496,15 @@
   <dimension ref="A2:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="B5:C5"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="19.21875" customWidth="1"/>
+    <col min="1" max="1" width="19.21875" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.21875" bestFit="1" customWidth="1"/>
@@ -624,6 +631,48 @@
       <c r="B5" t="s">
         <v>30</v>
       </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" t="s">
+        <v>31</v>
+      </c>
+      <c r="O5" t="s">
+        <v>31</v>
+      </c>
+      <c r="P5" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>